<commit_message>
update envelope archetypes to include more values
</commit_message>
<xml_diff>
--- a/cea/databases/SG/archetypes/CONSTRUCTION_STANDARD.xlsx
+++ b/cea/databases/SG/archetypes/CONSTRUCTION_STANDARD.xlsx
@@ -16,7 +16,6 @@
     <sheet name="ENVELOPE_ASSEMBLIES" sheetId="3" r:id="rId2"/>
     <sheet name="HVAC_ASSEMBLIES" sheetId="1" r:id="rId3"/>
     <sheet name="SUPPLY_ASSEMBLIES" sheetId="8" r:id="rId4"/>
-    <sheet name="EMISSION_INTENSITY" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="65">
   <si>
     <t>type_hs</t>
   </si>
@@ -117,45 +116,6 @@
     <t>Hs_bg</t>
   </si>
   <si>
-    <t>W_e_ag_kgm2</t>
-  </si>
-  <si>
-    <t>W_e_bg_kgm2</t>
-  </si>
-  <si>
-    <t>W_i_ag_kgm2</t>
-  </si>
-  <si>
-    <t>W_i_bg_kgm2</t>
-  </si>
-  <si>
-    <t>Win_kgm2</t>
-  </si>
-  <si>
-    <t>F_i_kgm2</t>
-  </si>
-  <si>
-    <t>F_e_kgm2</t>
-  </si>
-  <si>
-    <t>R_kgm2</t>
-  </si>
-  <si>
-    <t>Tech_kgm2</t>
-  </si>
-  <si>
-    <t>Exca_kgm2</t>
-  </si>
-  <si>
-    <t>Mobi_kgm2</t>
-  </si>
-  <si>
-    <t>Reference</t>
-  </si>
-  <si>
-    <t>SIA2040: Residential (current values: Top-Down Method)</t>
-  </si>
-  <si>
     <t>Concrete and Masonry with outdoor  corridors</t>
   </si>
   <si>
@@ -256,6 +216,15 @@
   </si>
   <si>
     <t>type_base</t>
+  </si>
+  <si>
+    <t>type_part</t>
+  </si>
+  <si>
+    <t>WALL_AS3</t>
+  </si>
+  <si>
+    <t>WALL_AS6</t>
   </si>
 </sst>
 </file>
@@ -769,7 +738,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -790,26 +759,6 @@
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1160,57 +1109,57 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>50</v>
+        <v>31</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="20">
+      <c r="A2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="12">
         <v>1900</v>
       </c>
-      <c r="D2" s="20">
+      <c r="D2" s="12">
         <v>2020</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="20">
+      <c r="A3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="12">
         <v>1900</v>
       </c>
-      <c r="D3" s="20">
+      <c r="D3" s="12">
         <v>2020</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="20">
+      <c r="A4" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="12">
         <v>1900</v>
       </c>
-      <c r="D4" s="20">
+      <c r="D4" s="12">
         <v>2020</v>
       </c>
     </row>
@@ -1221,13 +1170,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
+      <selection pane="bottomRight" activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1236,18 +1185,18 @@
     <col min="2" max="2" width="19.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.28515625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="7.140625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="10.85546875" style="3" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="7" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.28515625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="7.140625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="10.85546875" style="3" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>9</v>
@@ -1262,90 +1211,93 @@
         <v>7</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>71</v>
-      </c>
       <c r="H1" s="4" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>46</v>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="J2" s="2">
+      <c r="H2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" s="2">
         <v>0.9</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="2">
         <v>0.25</v>
       </c>
-      <c r="L2" s="5">
+      <c r="M2" s="5">
         <v>0</v>
-      </c>
-      <c r="M2" s="2">
-        <v>1</v>
       </c>
       <c r="N2" s="2">
         <v>1</v>
       </c>
       <c r="O2" s="2">
-        <v>0.28999999999999998</v>
+        <v>1</v>
       </c>
       <c r="P2" s="2">
         <v>0.28999999999999998</v>
@@ -1356,53 +1308,56 @@
       <c r="R2" s="2">
         <v>0.28999999999999998</v>
       </c>
-      <c r="T2" s="7"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>47</v>
+      <c r="S2" s="2">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="U2" s="7"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="I3" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="J3" s="2">
+      <c r="H3" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="K3" s="2">
         <v>0.9</v>
       </c>
-      <c r="K3" s="2">
+      <c r="L3" s="2">
         <v>0.84</v>
       </c>
-      <c r="L3" s="5">
+      <c r="M3" s="5">
         <v>0</v>
-      </c>
-      <c r="M3" s="2">
-        <v>1</v>
       </c>
       <c r="N3" s="2">
         <v>1</v>
       </c>
       <c r="O3" s="2">
-        <v>0.28999999999999998</v>
+        <v>1</v>
       </c>
       <c r="P3" s="2">
         <v>0.28999999999999998</v>
@@ -1413,53 +1368,56 @@
       <c r="R3" s="2">
         <v>0.28999999999999998</v>
       </c>
-      <c r="T3" s="7"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>48</v>
+      <c r="S3" s="2">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="U3" s="7"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="J4" s="2">
+      <c r="H4" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="K4" s="2">
         <v>0.9</v>
       </c>
-      <c r="K4" s="2">
+      <c r="L4" s="2">
         <v>0.84</v>
       </c>
-      <c r="L4" s="5">
+      <c r="M4" s="5">
         <v>0</v>
       </c>
-      <c r="M4" s="2">
+      <c r="N4" s="2">
         <v>1</v>
       </c>
-      <c r="N4" s="2">
+      <c r="O4" s="2">
         <v>0</v>
-      </c>
-      <c r="O4" s="2">
-        <v>0.59</v>
       </c>
       <c r="P4" s="2">
         <v>0.59</v>
@@ -1468,6 +1426,9 @@
         <v>0.59</v>
       </c>
       <c r="R4" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="S4" s="2">
         <v>0.59</v>
       </c>
     </row>
@@ -1502,7 +1463,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -1533,23 +1494,23 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>20</v>
@@ -1565,23 +1526,23 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>47</v>
+      <c r="A3" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>20</v>
@@ -1597,23 +1558,23 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>20</v>
@@ -1656,7 +1617,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -1672,54 +1633,54 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>46</v>
+      <c r="A2" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>47</v>
+      <c r="A3" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>48</v>
+      <c r="A4" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
     </row>
     <row r="1048559" spans="5:5" x14ac:dyDescent="0.25">
@@ -1728,200 +1689,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" style="15" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="52.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="10"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="11">
-        <v>36</v>
-      </c>
-      <c r="C2" s="11">
-        <v>35</v>
-      </c>
-      <c r="D2" s="11">
-        <v>34</v>
-      </c>
-      <c r="E2" s="11">
-        <v>21</v>
-      </c>
-      <c r="F2" s="11">
-        <v>123</v>
-      </c>
-      <c r="G2" s="11">
-        <v>110</v>
-      </c>
-      <c r="H2" s="11">
-        <v>113</v>
-      </c>
-      <c r="I2" s="11">
-        <v>113</v>
-      </c>
-      <c r="J2" s="11">
-        <v>32</v>
-      </c>
-      <c r="K2" s="11">
-        <v>135</v>
-      </c>
-      <c r="L2" s="12">
-        <v>16</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="11">
-        <v>57</v>
-      </c>
-      <c r="C3" s="11">
-        <v>71</v>
-      </c>
-      <c r="D3" s="11">
-        <v>34</v>
-      </c>
-      <c r="E3" s="11">
-        <v>21</v>
-      </c>
-      <c r="F3" s="11">
-        <v>69</v>
-      </c>
-      <c r="G3" s="11">
-        <v>91</v>
-      </c>
-      <c r="H3" s="11">
-        <v>104</v>
-      </c>
-      <c r="I3" s="11">
-        <v>113</v>
-      </c>
-      <c r="J3" s="11">
-        <v>32</v>
-      </c>
-      <c r="K3" s="11">
-        <v>135</v>
-      </c>
-      <c r="L3" s="12">
-        <v>16</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="11">
-        <v>112</v>
-      </c>
-      <c r="C4" s="11">
-        <v>188</v>
-      </c>
-      <c r="D4" s="11">
-        <v>73</v>
-      </c>
-      <c r="E4" s="11">
-        <v>16</v>
-      </c>
-      <c r="F4" s="11">
-        <v>85</v>
-      </c>
-      <c r="G4" s="11">
-        <v>75</v>
-      </c>
-      <c r="H4" s="11">
-        <v>180</v>
-      </c>
-      <c r="I4" s="11">
-        <v>78</v>
-      </c>
-      <c r="J4" s="11">
-        <v>32</v>
-      </c>
-      <c r="K4" s="11">
-        <v>135</v>
-      </c>
-      <c r="L4" s="12">
-        <v>16</v>
-      </c>
-      <c r="M4" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update year start and end to 1700	and 2040
</commit_message>
<xml_diff>
--- a/cea/databases/SG/archetypes/CONSTRUCTION_STANDARD.xlsx
+++ b/cea/databases/SG/archetypes/CONSTRUCTION_STANDARD.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JimenoF\Documents\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\SG\archetypes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\SG\archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="19605" tabRatio="785" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="470" windowWidth="38400" windowHeight="19610" tabRatio="785"/>
   </bookViews>
   <sheets>
     <sheet name="STANDARD_DEFINITION" sheetId="10" r:id="rId1"/>
@@ -1095,19 +1095,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>33</v>
       </c>
@@ -1129,13 +1129,13 @@
         <v>28</v>
       </c>
       <c r="C2" s="12">
-        <v>1900</v>
+        <v>1700</v>
       </c>
       <c r="D2" s="12">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>34</v>
       </c>
@@ -1143,13 +1143,13 @@
         <v>29</v>
       </c>
       <c r="C3" s="12">
-        <v>1900</v>
+        <v>1700</v>
       </c>
       <c r="D3" s="12">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>35</v>
       </c>
@@ -1157,10 +1157,10 @@
         <v>30</v>
       </c>
       <c r="C4" s="12">
-        <v>1900</v>
+        <v>1700</v>
       </c>
       <c r="D4" s="12">
-        <v>2020</v>
+        <v>2040</v>
       </c>
     </row>
   </sheetData>
@@ -1172,29 +1172,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="12.28515625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="14" width="7.140625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="19" width="10.85546875" style="3" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="7" width="12.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.26953125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="13.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="7.1796875" style="3" customWidth="1"/>
+    <col min="15" max="15" width="10.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="10.81640625" style="3" customWidth="1"/>
+    <col min="20" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>33</v>
       </c>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="U2" s="7"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>34</v>
       </c>
@@ -1373,7 +1373,7 @@
       </c>
       <c r="U3" s="7"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>35</v>
       </c>
@@ -1446,22 +1446,22 @@
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="12.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.81640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>33</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>34</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>35</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="1048560" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="1048560" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E1048560" s="2"/>
     </row>
   </sheetData>
@@ -1606,16 +1606,16 @@
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.54296875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>33</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>34</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>35</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="1048559" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="1048559" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E1048559" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update construction standard singapore to contain values in typology
</commit_message>
<xml_diff>
--- a/cea/databases/SG/archetypes/CONSTRUCTION_STANDARD.xlsx
+++ b/cea/databases/SG/archetypes/CONSTRUCTION_STANDARD.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\SG\archetypes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JimenoF\Documents\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\SG\archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="470" windowWidth="38400" windowHeight="19610" tabRatio="785"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="19605" tabRatio="785"/>
   </bookViews>
   <sheets>
     <sheet name="STANDARD_DEFINITION" sheetId="10" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="67">
   <si>
     <t>type_hs</t>
   </si>
@@ -225,6 +225,12 @@
   </si>
   <si>
     <t>WALL_AS6</t>
+  </si>
+  <si>
+    <t>STANDARD4</t>
+  </si>
+  <si>
+    <t>STANDARD5</t>
   </si>
 </sst>
 </file>
@@ -1093,21 +1099,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.81640625" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
@@ -1121,7 +1127,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>33</v>
       </c>
@@ -1129,13 +1135,13 @@
         <v>28</v>
       </c>
       <c r="C2" s="12">
-        <v>1700</v>
+        <v>1000</v>
       </c>
       <c r="D2" s="12">
         <v>2040</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>34</v>
       </c>
@@ -1143,13 +1149,13 @@
         <v>29</v>
       </c>
       <c r="C3" s="12">
-        <v>1700</v>
+        <v>1000</v>
       </c>
       <c r="D3" s="12">
         <v>2040</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>35</v>
       </c>
@@ -1157,9 +1163,37 @@
         <v>30</v>
       </c>
       <c r="C4" s="12">
-        <v>1700</v>
+        <v>1000</v>
       </c>
       <c r="D4" s="12">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="12">
+        <v>1000</v>
+      </c>
+      <c r="D5" s="12">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="12">
+        <v>1000</v>
+      </c>
+      <c r="D6" s="12">
         <v>2040</v>
       </c>
     </row>
@@ -1170,31 +1204,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I8" sqref="I8"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6:S6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="12.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="12.26953125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="13.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="14" width="7.1796875" style="3" customWidth="1"/>
-    <col min="15" max="15" width="10.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="19" width="10.81640625" style="3" customWidth="1"/>
-    <col min="20" max="16384" width="9.1796875" style="1"/>
+    <col min="5" max="7" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.28515625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="7.140625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="10.85546875" style="3" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
@@ -1253,7 +1287,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>33</v>
       </c>
@@ -1313,7 +1347,7 @@
       </c>
       <c r="U2" s="7"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>34</v>
       </c>
@@ -1373,7 +1407,7 @@
       </c>
       <c r="U3" s="7"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>35</v>
       </c>
@@ -1429,6 +1463,124 @@
         <v>0.59</v>
       </c>
       <c r="S4" s="2">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0.84</v>
+      </c>
+      <c r="M5" s="5">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
+        <v>1</v>
+      </c>
+      <c r="O5" s="2">
+        <v>0</v>
+      </c>
+      <c r="P5" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="R5" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="S5" s="2">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0.84</v>
+      </c>
+      <c r="M6" s="5">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2">
+        <v>1</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0</v>
+      </c>
+      <c r="P6" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="R6" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="S6" s="2">
         <v>0.59</v>
       </c>
     </row>
@@ -1443,25 +1595,25 @@
   <dimension ref="A1:J1048560"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="B6" sqref="B6:J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.26953125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.81640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="12.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
@@ -1493,7 +1645,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>33</v>
       </c>
@@ -1525,7 +1677,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>34</v>
       </c>
@@ -1557,7 +1709,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>35</v>
       </c>
@@ -1589,7 +1741,71 @@
         <v>21</v>
       </c>
     </row>
-    <row r="1048560" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1048560" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E1048560" s="2"/>
     </row>
   </sheetData>
@@ -1603,19 +1819,19 @@
   <dimension ref="A1:E1048559"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.26953125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
@@ -1632,7 +1848,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>33</v>
       </c>
@@ -1649,7 +1865,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>34</v>
       </c>
@@ -1666,7 +1882,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>35</v>
       </c>
@@ -1683,7 +1899,41 @@
         <v>38</v>
       </c>
     </row>
-    <row r="1048559" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1048559" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E1048559" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixes in the database
removed repeated construction_standards and updated descriptions to be more intuitive. Removed U_base from WALL (ENVELOPE ASSEMBLY)
</commit_message>
<xml_diff>
--- a/cea/databases/SG/archetypes/CONSTRUCTION_STANDARD.xlsx
+++ b/cea/databases/SG/archetypes/CONSTRUCTION_STANDARD.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JimenoF\Documents\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\SG\archetypes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis.santos\Documents\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\SG\archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132FC95B-4B67-4BBC-880C-7EC0EB483714}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="19605" tabRatio="785"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="785" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STANDARD_DEFINITION" sheetId="10" r:id="rId1"/>
@@ -17,10 +18,19 @@
     <sheet name="HVAC_ASSEMBLIES" sheetId="1" r:id="rId3"/>
     <sheet name="SUPPLY_ASSEMBLIES" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="65">
   <si>
     <t>type_hs</t>
   </si>
@@ -116,15 +126,6 @@
     <t>Hs_bg</t>
   </si>
   <si>
-    <t>Concrete and Masonry with outdoor  corridors</t>
-  </si>
-  <si>
-    <t>Concrete and Masonry with indoor  corridors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Concrete, Masonry and Rainscreens </t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -227,16 +228,19 @@
     <t>WALL_AS6</t>
   </si>
   <si>
-    <t>STANDARD4</t>
-  </si>
-  <si>
-    <t>STANDARD5</t>
+    <t>Concrete and Masonry - commercial</t>
+  </si>
+  <si>
+    <t>Concrete and Masonry - residential, reduced conditioned areas</t>
+  </si>
+  <si>
+    <t>Concrete and Masonry - residential, increased conditioned areas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -756,9 +760,6 @@
     <xf numFmtId="49" fontId="17" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -769,14 +770,17 @@
     <xf numFmtId="49" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="17" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1098,102 +1102,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.7109375" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>37</v>
+        <v>28</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="12">
+      <c r="A2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="10">
         <v>1000</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="10">
         <v>2040</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="12">
+      <c r="A3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="10">
         <v>1000</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="10">
         <v>2040</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="12">
+      <c r="A4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="10">
         <v>1000</v>
       </c>
-      <c r="D4" s="12">
-        <v>2040</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="12">
-        <v>1000</v>
-      </c>
-      <c r="D5" s="12">
-        <v>2040</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="12">
-        <v>1000</v>
-      </c>
-      <c r="D6" s="12">
+      <c r="D4" s="10">
         <v>2040</v>
       </c>
     </row>
@@ -1203,19 +1179,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6:S6"/>
+      <selection pane="bottomRight" activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" style="3" bestFit="1" customWidth="1"/>
@@ -1230,7 +1206,7 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>9</v>
@@ -1245,16 +1221,16 @@
         <v>7</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>4</v>
@@ -1288,299 +1264,181 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>33</v>
+      <c r="A2" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="K2" s="2">
+      <c r="K2" s="11">
         <v>0.9</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="11">
         <v>0.25</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2" s="12">
         <v>0</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="11">
         <v>1</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2" s="11">
         <v>1</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2" s="11">
         <v>0.28999999999999998</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="Q2" s="11">
         <v>0.28999999999999998</v>
       </c>
-      <c r="R2" s="2">
+      <c r="R2" s="11">
         <v>0.28999999999999998</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S2" s="11">
         <v>0.28999999999999998</v>
       </c>
-      <c r="U2" s="7"/>
+      <c r="U2" s="6"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>34</v>
+      <c r="A3" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="J3" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="F3" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="K3" s="2">
+      <c r="K3" s="11">
         <v>0.9</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="11">
         <v>0.84</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="12">
         <v>0</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="11">
         <v>1</v>
       </c>
-      <c r="O3" s="2">
+      <c r="O3" s="11">
         <v>1</v>
       </c>
-      <c r="P3" s="2">
+      <c r="P3" s="11">
         <v>0.28999999999999998</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="Q3" s="11">
         <v>0.28999999999999998</v>
       </c>
-      <c r="R3" s="2">
+      <c r="R3" s="11">
         <v>0.28999999999999998</v>
       </c>
-      <c r="S3" s="2">
+      <c r="S3" s="11">
         <v>0.28999999999999998</v>
       </c>
-      <c r="U3" s="7"/>
+      <c r="U3" s="6"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>35</v>
+      <c r="A4" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" s="10" t="s">
+      <c r="F4" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="J4" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="K4" s="2">
+      <c r="K4" s="11">
         <v>0.9</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="11">
         <v>0.84</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="12">
         <v>0</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="11">
         <v>1</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4" s="11">
         <v>0</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4" s="11">
         <v>0.59</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="Q4" s="11">
         <v>0.59</v>
       </c>
-      <c r="R4" s="2">
+      <c r="R4" s="11">
         <v>0.59</v>
       </c>
-      <c r="S4" s="2">
-        <v>0.59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="K5" s="2">
-        <v>0.9</v>
-      </c>
-      <c r="L5" s="2">
-        <v>0.84</v>
-      </c>
-      <c r="M5" s="5">
-        <v>0</v>
-      </c>
-      <c r="N5" s="2">
-        <v>1</v>
-      </c>
-      <c r="O5" s="2">
-        <v>0</v>
-      </c>
-      <c r="P5" s="2">
-        <v>0.59</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>0.59</v>
-      </c>
-      <c r="R5" s="2">
-        <v>0.59</v>
-      </c>
-      <c r="S5" s="2">
-        <v>0.59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="K6" s="2">
-        <v>0.9</v>
-      </c>
-      <c r="L6" s="2">
-        <v>0.84</v>
-      </c>
-      <c r="M6" s="5">
-        <v>0</v>
-      </c>
-      <c r="N6" s="2">
-        <v>1</v>
-      </c>
-      <c r="O6" s="2">
-        <v>0</v>
-      </c>
-      <c r="P6" s="2">
-        <v>0.59</v>
-      </c>
-      <c r="Q6" s="2">
-        <v>0.59</v>
-      </c>
-      <c r="R6" s="2">
-        <v>0.59</v>
-      </c>
-      <c r="S6" s="2">
+      <c r="S4" s="11">
         <v>0.59</v>
       </c>
     </row>
@@ -1591,16 +1449,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1048560"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:J1048558"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:J6"/>
+      <selection activeCell="C2" sqref="C2:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" style="3" bestFit="1" customWidth="1"/>
@@ -1615,7 +1473,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -1646,167 +1504,103 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>33</v>
+      <c r="A2" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>34</v>
+      <c r="A3" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>35</v>
+      <c r="A4" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="E4" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="1048560" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E1048560" s="2"/>
+    <row r="1048558" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1048558" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1815,25 +1609,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1048559"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:E1048557"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -1849,92 +1644,58 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>33</v>
+      <c r="A2" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>34</v>
+      <c r="A3" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>38</v>
-      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="1048559" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E1048559" s="2"/>
+    <row r="1048557" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1048557" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>